<commit_message>
slowly add code to create folder N+1 for document download
</commit_message>
<xml_diff>
--- a/Folder Creation - Willy/Project_Notebook.xlsx
+++ b/Folder Creation - Willy/Project_Notebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoelwill\Documents\UiPath\.repositories\Everest Git\Folder Creation - Willy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8286CC3C-9384-43DF-83C4-470CBCF3BE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB82C7D-3BA6-491E-A262-ADFA1834E4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <definedName name="FileNameNoExtension">File!$B$11</definedName>
     <definedName name="FileNoextNoRev">File!$B$12</definedName>
     <definedName name="FirstName">Text!$B$15</definedName>
-    <definedName name="Folder">File!$B$16</definedName>
+    <definedName name="Folder">File!$B$17</definedName>
     <definedName name="FullFileName_Input">File!$B$6</definedName>
     <definedName name="Int">Number!$B$6</definedName>
     <definedName name="LastMonthEndDate">Date!$C$14</definedName>
@@ -49,13 +49,14 @@
     <definedName name="LastWeekSunday">Date!$D$13</definedName>
     <definedName name="Length">Text!$B$6</definedName>
     <definedName name="LowerCase">Text!$B$8</definedName>
+    <definedName name="NewFolder">File!$B$17</definedName>
     <definedName name="NewRevision">File!$B$14</definedName>
-    <definedName name="NewRevisionFileName">File!$B$21</definedName>
+    <definedName name="NewRevisionFileName">File!$B$22</definedName>
     <definedName name="Number_Input">Number!$B$4</definedName>
     <definedName name="NumberText_Input">Number!$B$11</definedName>
     <definedName name="preferred_date_format">Date!$B$6</definedName>
     <definedName name="ReformattedDate">Date!$B$31</definedName>
-    <definedName name="ReformattedFileName">File!$B$20</definedName>
+    <definedName name="ReformattedFileName">File!$B$21</definedName>
     <definedName name="ReformattedNumber">Number!$B$15</definedName>
     <definedName name="Replace">Text!$B$11</definedName>
     <definedName name="Result">Text!$B$12</definedName>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="95">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -355,19 +356,25 @@
     <t>C:\Users\hoelwill\Documents\UiPath\Document masterlist\CJA\CJA Document Masterlist Everest Rev 0.xlsx</t>
   </si>
   <si>
-    <t>Revision</t>
-  </si>
-  <si>
     <t>File name no extension no revision</t>
   </si>
   <si>
-    <t>Revision + 1</t>
-  </si>
-  <si>
     <t>CM Name</t>
   </si>
   <si>
     <t>Universal File Name</t>
+  </si>
+  <si>
+    <t>Revision N</t>
+  </si>
+  <si>
+    <t>Revision N + 1</t>
+  </si>
+  <si>
+    <t>Reformatted File Name N+1:</t>
+  </si>
+  <si>
+    <t>New Folder N + 1</t>
   </si>
 </sst>
 </file>
@@ -552,7 +559,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -644,28 +651,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -765,6 +750,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -797,25 +835,25 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="5" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" applyNumberFormat="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" applyNumberFormat="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
@@ -833,7 +871,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -855,10 +893,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -922,9 +956,22 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Bottom Border" xfId="16" xr:uid="{79AD1433-2737-4ED4-9B85-92BE82D167F0}"/>
@@ -1522,20 +1569,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
@@ -1569,7 +1616,7 @@
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="28" t="str">
+      <c r="B8" s="26" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
         <v>2023-05-19</v>
       </c>
@@ -1578,7 +1625,7 @@
       <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="28" t="str">
+      <c r="B9" s="26" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
         <v>2023-05-23</v>
       </c>
@@ -1587,7 +1634,7 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="29" t="str">
+      <c r="B10" s="27" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
         <v>20230512</v>
       </c>
@@ -1596,7 +1643,7 @@
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="28" t="str">
+      <c r="B12" s="26" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
         <v>2023-05-12</v>
       </c>
@@ -1605,15 +1652,15 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="28" t="str">
+      <c r="B13" s="26" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-6, preferred_date_format)</f>
         <v>2023-05-01</v>
       </c>
-      <c r="C13" s="28" t="str">
+      <c r="C13" s="26" t="str">
         <f ca="1">TEXT(LastWeekMonday+4, preferred_date_format)</f>
         <v>2023-05-05</v>
       </c>
-      <c r="D13" s="30" t="str">
+      <c r="D13" s="28" t="str">
         <f ca="1">TEXT(LastWeekFriday+2, preferred_date_format)</f>
         <v>2023-05-07</v>
       </c>
@@ -1622,11 +1669,11 @@
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="28" t="str">
+      <c r="B14" s="26" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1), preferred_date_format)</f>
         <v>2023-04-01</v>
       </c>
-      <c r="C14" s="28" t="str">
+      <c r="C14" s="26" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), 0), preferred_date_format)</f>
         <v>2023-04-30</v>
       </c>
@@ -1635,23 +1682,23 @@
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="28" t="str">
+      <c r="B15" s="26" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1), preferred_date_format)</f>
         <v>2023-05-01</v>
       </c>
-      <c r="C15" s="28" t="str">
+      <c r="C15" s="26" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1), preferred_date_format)</f>
         <v>2023-05-31</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
@@ -1663,11 +1710,11 @@
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
@@ -1776,7 +1823,7 @@
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="29" t="s">
         <v>85</v>
       </c>
       <c r="B30" t="str">
@@ -1826,30 +1873,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>65</v>
       </c>
       <c r="C4" t="s">
@@ -1882,7 +1929,7 @@
       <c r="E5" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="17" t="str">
+      <c r="F5" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D5,Text_Input)+LEN(D5), IFERROR(FIND(IF(E5="",CHAR(10),E5),Text_Input,FIND(D5,Text_Input)+LEN(D5)),LEN(Text_Input)+1)-FIND(D5,Text_Input)-LEN(D5)))</f>
         <v>C.</v>
       </c>
@@ -1901,7 +1948,7 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="17" t="str">
+      <c r="F6" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D6,Text_Input)+LEN(D6), IFERROR(FIND(IF(E6="",CHAR(10),E6),Text_Input,FIND(D6,Text_Input)+LEN(D6)),LEN(Text_Input)+1)-FIND(D6,Text_Input)-LEN(D6)))</f>
         <v>C. Doe</v>
       </c>
@@ -1920,7 +1967,7 @@
       <c r="E7" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="17" t="str">
+      <c r="F7" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D7,Text_Input)+LEN(D7), IFERROR(FIND(IF(E7="",CHAR(10),E7),Text_Input,FIND(D7,Text_Input)+LEN(D7)),LEN(Text_Input)+1)-FIND(D7,Text_Input)-LEN(D7)))</f>
         <v>John C.</v>
       </c>
@@ -1939,7 +1986,7 @@
       <c r="D8" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="17" t="str">
+      <c r="F8" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D8,Text_Input)+LEN(D8), IFERROR(FIND(IF(E8="",CHAR(10),E8),Text_Input,FIND(D8,Text_Input)+LEN(D8)),LEN(Text_Input)+1)-FIND(D8,Text_Input)-LEN(D8)))</f>
         <v>Doe</v>
       </c>
@@ -1948,7 +1995,7 @@
       <c r="C9" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="17" t="str">
+      <c r="F9" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D9,Text_Input)+LEN(D9), IFERROR(FIND(IF(E9="",CHAR(10),E9),Text_Input,FIND(D9,Text_Input)+LEN(D9)),LEN(Text_Input)+1)-FIND(D9,Text_Input)-LEN(D9)))</f>
         <v>John C. Doe</v>
       </c>
@@ -2060,32 +2107,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>3.1415929999999999</v>
       </c>
     </row>
@@ -2118,10 +2165,10 @@
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="34"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
@@ -2182,10 +2229,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B15AA95-D2AA-4AD6-8E83-DBFAD20B8498}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2196,141 +2243,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="36"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="34"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="39" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="41"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="6" t="str">
+      <c r="B8" s="41" t="str">
         <f>TRIM(RIGHT(SUBSTITUTE(B6,"\",REPT(" ",LEN(B6))),LEN(B6)))</f>
         <v>CJA Document Masterlist Everest Rev 0.xlsx</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="6" t="str">
+      <c r="B9" s="41" t="str">
         <f>TRIM(RIGHT(SUBSTITUTE(B8,".",REPT(" ",LEN(B8))),LEN(B8)))</f>
         <v>xlsx</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" s="6" t="str">
+      <c r="A10" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="41" t="str">
         <f>RIGHT(FileNoextNoRev, LEN(FileNoextNoRev)-4)</f>
         <v xml:space="preserve">Document Masterlist Everest Rev </v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="6" t="str">
+      <c r="B11" s="41" t="str">
         <f>LEFT(B8, LEN(B8)-LEN(B9)-1)</f>
         <v>CJA Document Masterlist Everest Rev 0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="6" t="str">
+      <c r="A12" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="41" t="str">
         <f>LEFT(FileName,36)</f>
         <v xml:space="preserve">CJA Document Masterlist Everest Rev </v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="6" t="str">
+      <c r="A13" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="41" t="str">
         <f>RIGHT(B11, LEN(B11)-LEN(B12))</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="40">
+      <c r="A14" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="43">
         <f>B13+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="40" t="str">
+      <c r="A15" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="43" t="str">
         <f>LEFT(FileNoextNoRev,3)</f>
         <v>CJA</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="9" t="str">
+      <c r="B16" s="41" t="str">
         <f>LEFT(B6, LEN(B6)-LEN(B8))</f>
         <v>C:\Users\hoelwill\Documents\UiPath\Document masterlist\CJA\</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" t="str">
-        <f>FileNameNoExtension &amp; "." &amp; FileExtension</f>
-        <v>CJA Document Masterlist Everest Rev 0.xlsx</v>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="45" t="str">
+        <f>LEFT(B6, LEN(B6)-LEN(B8))&amp;"Everest Download Rev "&amp;NewRevision&amp;"\"</f>
+        <v>C:\Users\hoelwill\Documents\UiPath\Document masterlist\CJA\Everest Download Rev 1\</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -2338,6 +2385,15 @@
         <v>57</v>
       </c>
       <c r="B21" t="str">
+        <f>FileNameNoExtension &amp; "." &amp; FileExtension</f>
+        <v>CJA Document Masterlist Everest Rev 0.xlsx</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" t="str">
         <f>CMName&amp;" "&amp;UniversalDMSName&amp;NewRevision&amp;"."&amp;FileExtension</f>
         <v>CJA Document Masterlist Everest Rev 1.xlsx</v>
       </c>
@@ -2369,105 +2425,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22"/>
+      <c r="A1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="35" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="37" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="22" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="21"/>
-      <c r="D4" s="19"/>
+      <c r="A4" s="19"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>71</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="21" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
+      <c r="A8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
+      <c r="A9" s="19"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
+      <c r="A10" s="19"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
+      <c r="A11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
+      <c r="A12" s="19"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
+      <c r="A13" s="19"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
+      <c r="A14" s="19"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
+      <c r="A15" s="19"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
+      <c r="A16" s="19"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
+      <c r="A17" s="19"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
+      <c r="A18" s="19"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21"/>
+      <c r="A19" s="19"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="21"/>
+      <c r="A20" s="19"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="21"/>
+      <c r="A21" s="19"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="21"/>
+      <c r="A22" s="19"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="18" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="21" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="21" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="21" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="21" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small step update at 11:38am 16May23
</commit_message>
<xml_diff>
--- a/Folder Creation - Willy/Project_Notebook.xlsx
+++ b/Folder Creation - Willy/Project_Notebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoelwill\Documents\UiPath\.repositories\Everest Git\Folder Creation - Willy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hp.sharepoint.com/teams/MTOBot-a-thon2022/Shared Documents/06- Real time Alert of HP Document Revs/Everest Playground/Folder Creation - Willy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB82C7D-3BA6-491E-A262-ADFA1834E4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{472881D3-8293-4C1A-B8EF-34C858409D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="4" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
@@ -25,20 +25,23 @@
     <definedName name="_A2">Scratchpad!$A$2</definedName>
     <definedName name="_A3">Scratchpad!$A$3</definedName>
     <definedName name="CleanNumber">Number!$B$5</definedName>
-    <definedName name="CMName">File!$B$15</definedName>
+    <definedName name="CM_Folder_path">File!$B$17</definedName>
+    <definedName name="CMName">File!$B$16</definedName>
     <definedName name="Contains">Text!$B$13</definedName>
-    <definedName name="CurrentRevision">File!$B$13</definedName>
+    <definedName name="CurrentRevision">File!$B$14</definedName>
     <definedName name="Date_Input">Date!$B$4</definedName>
     <definedName name="DatePlusDays">Date!$B$8</definedName>
     <definedName name="DatePlusWorkingDays">Date!$B$9</definedName>
     <definedName name="DateText">Date!$B$19</definedName>
     <definedName name="Days">Date!$B$7</definedName>
-    <definedName name="FileExtension">File!$B$9</definedName>
+    <definedName name="FileExtension">File!$B$10</definedName>
     <definedName name="FileName">File!$B$8</definedName>
-    <definedName name="FileNameNoExtension">File!$B$11</definedName>
+    <definedName name="FileNameNoExtension">File!$B$13</definedName>
     <definedName name="FileNoextNoRev">File!$B$12</definedName>
     <definedName name="FirstName">Text!$B$15</definedName>
-    <definedName name="Folder">File!$B$17</definedName>
+    <definedName name="Folder_path">File!$B$17</definedName>
+    <definedName name="Full_New_File_name">File!$B$20</definedName>
+    <definedName name="Full_New_File_Path">File!$B$21</definedName>
     <definedName name="FullFileName_Input">File!$B$6</definedName>
     <definedName name="Int">Number!$B$6</definedName>
     <definedName name="LastMonthEndDate">Date!$C$14</definedName>
@@ -49,14 +52,15 @@
     <definedName name="LastWeekSunday">Date!$D$13</definedName>
     <definedName name="Length">Text!$B$6</definedName>
     <definedName name="LowerCase">Text!$B$8</definedName>
-    <definedName name="NewFolder">File!$B$17</definedName>
-    <definedName name="NewRevision">File!$B$14</definedName>
-    <definedName name="NewRevisionFileName">File!$B$22</definedName>
+    <definedName name="New_DML_Name">File!$B$18</definedName>
+    <definedName name="New_SubFolder_Path">File!$B$19</definedName>
+    <definedName name="NewRevision">File!$B$15</definedName>
+    <definedName name="NewRevisionFileName">File!$B$9</definedName>
     <definedName name="Number_Input">Number!$B$4</definedName>
     <definedName name="NumberText_Input">Number!$B$11</definedName>
     <definedName name="preferred_date_format">Date!$B$6</definedName>
     <definedName name="ReformattedDate">Date!$B$31</definedName>
-    <definedName name="ReformattedFileName">File!$B$21</definedName>
+    <definedName name="ReformattedFileName">File!#REF!</definedName>
     <definedName name="ReformattedNumber">Number!$B$15</definedName>
     <definedName name="Replace">Text!$B$11</definedName>
     <definedName name="Result">Text!$B$12</definedName>
@@ -67,7 +71,7 @@
     <definedName name="Today">Date!$B$12</definedName>
     <definedName name="Trimmed">Text!$B$5</definedName>
     <definedName name="TwoDecimals">Number!$B$7</definedName>
-    <definedName name="UniversalDMSName">File!$B$10</definedName>
+    <definedName name="UniversalDMSName">File!$B$11</definedName>
     <definedName name="UpperCase">Text!$B$7</definedName>
     <definedName name="YYYYMMDD">Date!$B$10</definedName>
   </definedNames>
@@ -89,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -260,9 +264,6 @@
   </si>
   <si>
     <t>Folder</t>
-  </si>
-  <si>
-    <t>Reformatted File Name:</t>
   </si>
   <si>
     <t>Days</t>
@@ -353,9 +354,6 @@
 Note: All dates are formatted using TEXT() to avoid formatting issues that can occur due to differences in formatting preferences</t>
   </si>
   <si>
-    <t>C:\Users\hoelwill\Documents\UiPath\Document masterlist\CJA\CJA Document Masterlist Everest Rev 0.xlsx</t>
-  </si>
-  <si>
     <t>File name no extension no revision</t>
   </si>
   <si>
@@ -375,6 +373,18 @@
   </si>
   <si>
     <t>New Folder N + 1</t>
+  </si>
+  <si>
+    <t>Full New File Path N + 1</t>
+  </si>
+  <si>
+    <t>DML N+1 Full File Path</t>
+  </si>
+  <si>
+    <t>Full New File name N + 1</t>
+  </si>
+  <si>
+    <t>C:\Temp\Everest\Document masterlist\CJA\CJA Document Masterlist Everest Rev 0.xlsx</t>
   </si>
 </sst>
 </file>
@@ -932,30 +942,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -972,6 +958,30 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Bottom Border" xfId="16" xr:uid="{79AD1433-2737-4ED4-9B85-92BE82D167F0}"/>
@@ -1569,20 +1579,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
     </row>
     <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="A2" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
@@ -1593,20 +1603,20 @@
       </c>
       <c r="B4" s="2">
         <f ca="1">TODAY()</f>
-        <v>45058</v>
+        <v>45062</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
         <v>83</v>
-      </c>
-      <c r="B6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1614,20 +1624,20 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="26" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
-        <v>2023-05-19</v>
+        <v>2023-05-23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="26" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
-        <v>2023-05-23</v>
+        <v>2023-05-25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1636,7 +1646,7 @@
       </c>
       <c r="B10" s="27" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
-        <v>20230512</v>
+        <v>20230516</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1645,7 +1655,7 @@
       </c>
       <c r="B12" s="26" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
-        <v>2023-05-12</v>
+        <v>2023-05-16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -1654,15 +1664,15 @@
       </c>
       <c r="B13" s="26" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-6, preferred_date_format)</f>
-        <v>2023-05-01</v>
+        <v>2023-05-08</v>
       </c>
       <c r="C13" s="26" t="str">
         <f ca="1">TEXT(LastWeekMonday+4, preferred_date_format)</f>
-        <v>2023-05-05</v>
+        <v>2023-05-12</v>
       </c>
       <c r="D13" s="28" t="str">
         <f ca="1">TEXT(LastWeekFriday+2, preferred_date_format)</f>
-        <v>2023-05-07</v>
+        <v>2023-05-14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -1693,12 +1703,12 @@
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
@@ -1710,11 +1720,11 @@
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
@@ -1824,7 +1834,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" t="str">
         <f>preferred_date_format</f>
@@ -1860,7 +1870,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1873,43 +1883,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="A2" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1921,13 +1931,13 @@
         <v>John C. Doe</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D5,Text_Input)+LEN(D5), IFERROR(FIND(IF(E5="",CHAR(10),E5),Text_Input,FIND(D5,Text_Input)+LEN(D5)),LEN(Text_Input)+1)-FIND(D5,Text_Input)-LEN(D5)))</f>
@@ -1943,7 +1953,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -1962,10 +1972,10 @@
         <v>JOHN C. DOE</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D7,Text_Input)+LEN(D7), IFERROR(FIND(IF(E7="",CHAR(10),E7),Text_Input,FIND(D7,Text_Input)+LEN(D7)),LEN(Text_Input)+1)-FIND(D7,Text_Input)-LEN(D7)))</f>
@@ -1981,10 +1991,10 @@
         <v>john c. doe</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D8,Text_Input)+LEN(D8), IFERROR(FIND(IF(E8="",CHAR(10),E8),Text_Input,FIND(D8,Text_Input)+LEN(D8)),LEN(Text_Input)+1)-FIND(D8,Text_Input)-LEN(D8)))</f>
@@ -1993,7 +2003,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D9,Text_Input)+LEN(D9), IFERROR(FIND(IF(E9="",CHAR(10),E9),Text_Input,FIND(D9,Text_Input)+LEN(D9)),LEN(Text_Input)+1)-FIND(D9,Text_Input)-LEN(D9)))</f>
@@ -2008,7 +2018,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -2019,7 +2029,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2031,7 +2041,7 @@
         <v>Mary C. Doe</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2043,12 +2053,12 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -2060,7 +2070,7 @@
         <v>John C.</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -2072,12 +2082,12 @@
         <v>Doe</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2107,18 +2117,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="43"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="36"/>
+      <c r="A2" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="44"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
     </row>
@@ -2138,7 +2148,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <f>VALUE(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Number_Input, CHAR(13), ""), CHAR(10), ""), CHAR(160), "")))</f>
@@ -2165,10 +2175,10 @@
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="34"/>
+      <c r="B9" s="42"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
@@ -2229,32 +2239,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B15AA95-D2AA-4AD6-8E83-DBFAD20B8498}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" customWidth="1"/>
+    <col min="2" max="2" width="143.54296875" customWidth="1"/>
     <col min="3" max="4" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="35"/>
+      <c r="A1" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="43"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="36"/>
+      <c r="A2" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="44"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
     </row>
@@ -2265,10 +2275,10 @@
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="42"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
@@ -2277,125 +2287,143 @@
       <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="39" t="s">
-        <v>87</v>
+      <c r="B6" s="31" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="41"/>
+      <c r="B7" s="33"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="41" t="str">
+      <c r="B8" s="33" t="str">
         <f>TRIM(RIGHT(SUBSTITUTE(B6,"\",REPT(" ",LEN(B6))),LEN(B6)))</f>
         <v>CJA Document Masterlist Everest Rev 0.xlsx</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" t="str">
+        <f>CMName&amp;" "&amp;UniversalDMSName&amp;NewRevision&amp;"."&amp;FileExtension</f>
+        <v>CJA Document Masterlist Everest Rev 1.xlsx</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="41" t="str">
+      <c r="B10" s="33" t="str">
         <f>TRIM(RIGHT(SUBSTITUTE(B8,".",REPT(" ",LEN(B8))),LEN(B8)))</f>
         <v>xlsx</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="41" t="str">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="33" t="str">
         <f>RIGHT(FileNoextNoRev, LEN(FileNoextNoRev)-4)</f>
         <v xml:space="preserve">Document Masterlist Everest Rev </v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="41" t="str">
-        <f>LEFT(B8, LEN(B8)-LEN(B9)-1)</f>
-        <v>CJA Document Masterlist Everest Rev 0</v>
-      </c>
-    </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="41" t="str">
+      <c r="A12" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="33" t="str">
         <f>LEFT(FileName,36)</f>
         <v xml:space="preserve">CJA Document Masterlist Everest Rev </v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="41" t="str">
-        <f>RIGHT(B11, LEN(B11)-LEN(B12))</f>
+      <c r="A13" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="33" t="str">
+        <f>LEFT(B8, LEN(B8)-LEN(B10)-1)</f>
+        <v>CJA Document Masterlist Everest Rev 0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="33" t="str">
+        <f>RIGHT(B13, LEN(B13)-LEN(B12))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="43">
-        <f>B13+1</f>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="35">
+        <f>B14+1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="43" t="str">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="35" t="str">
         <f>LEFT(FileNoextNoRev,3)</f>
         <v>CJA</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="42" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="41" t="str">
+      <c r="B17" s="33" t="str">
         <f>LEFT(B6, LEN(B6)-LEN(B8))</f>
-        <v>C:\Users\hoelwill\Documents\UiPath\Document masterlist\CJA\</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="44" t="s">
+        <v>C:\Temp\Everest\Document masterlist\CJA\</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="45" t="str">
+      <c r="B18" s="37" t="str">
+        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;UniversalDMSName&amp;" "&amp;NewRevision&amp;"."&amp;FileExtension</f>
+        <v>C:\Temp\Everest\Document masterlist\CJA\Document Masterlist Everest Rev  1.xlsx</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="33" t="str">
         <f>LEFT(B6, LEN(B6)-LEN(B8))&amp;"Everest Download Rev "&amp;NewRevision&amp;"\"</f>
-        <v>C:\Users\hoelwill\Documents\UiPath\Document masterlist\CJA\Everest Download Rev 1\</v>
+        <v>C:\Temp\Everest\Document masterlist\CJA\Everest Download Rev 1\</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="37" t="str">
+        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;"Everest Download Rev "&amp;NewRevision&amp;"\"&amp;CMName&amp;" "&amp;UniversalDMSName&amp;NewRevision</f>
+        <v>C:\Temp\Everest\Document masterlist\CJA\Everest Download Rev 1\CJA Document Masterlist Everest Rev 1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="str">
-        <f>FileNameNoExtension &amp; "." &amp; FileExtension</f>
-        <v>CJA Document Masterlist Everest Rev 0.xlsx</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A21" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="B22" t="str">
-        <f>CMName&amp;" "&amp;UniversalDMSName&amp;NewRevision&amp;"."&amp;FileExtension</f>
-        <v>CJA Document Masterlist Everest Rev 1.xlsx</v>
+      <c r="B21" s="37" t="str">
+        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;"Everest Download Rev "&amp;NewRevision&amp;"\"&amp;CMName&amp;" "&amp;UniversalDMSName&amp;NewRevision&amp;"."&amp;FileExtension</f>
+        <v>C:\Temp\Everest\Document masterlist\CJA\Everest Download Rev 1\CJA Document Masterlist Everest Rev 1.xlsx</v>
       </c>
     </row>
   </sheetData>
@@ -2429,12 +2457,12 @@
     </row>
     <row r="2" spans="1:5" ht="35" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="37" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2443,18 +2471,18 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2504,27 +2532,27 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2532,4 +2560,259 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B16600BB3F787049B388C7CFD7EEE15C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1a82d70544a00a602877de68251abad3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6a4c4680-0984-45cb-bb92-415d6e515dfa" xmlns:ns3="5f977c50-2d7a-484c-acbd-eec5a0379d47" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bed718036c05bd3ccaa54d95c4edc461" ns2:_="" ns3:_="">
+    <xsd:import namespace="6a4c4680-0984-45cb-bb92-415d6e515dfa"/>
+    <xsd:import namespace="5f977c50-2d7a-484c-acbd-eec5a0379d47"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6a4c4680-0984-45cb-bb92-415d6e515dfa" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="13" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="297f403b-2b63-43ad-9c62-fa967f2a159f" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="20" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5f977c50-2d7a-484c-acbd-eec5a0379d47" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{6c9727a0-cd4b-49c7-86ec-ad07e56e7520}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="5f977c50-2d7a-484c-acbd-eec5a0379d47">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5f977c50-2d7a-484c-acbd-eec5a0379d47" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6a4c4680-0984-45cb-bb92-415d6e515dfa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52D1FA1-5952-4DF9-A5CA-1242A1BDF162}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22DAA5A9-0921-4152-878F-F50DC19F8379}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{866B838F-E4C8-4E67-B277-878368C882B9}"/>
 </file>
</xml_diff>

<commit_message>
Small Step Update at 12:00pm 16May23 -Create New folder with revision N+1 for new document download and DML N+1 storage -Update Old DML to New DML with revision N+1 -Save another New DML N+1 in newly created folder -Delete Old DML for housekeeping purpose
</commit_message>
<xml_diff>
--- a/Folder Creation - Willy/Project_Notebook.xlsx
+++ b/Folder Creation - Willy/Project_Notebook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hp.sharepoint.com/teams/MTOBot-a-thon2022/Shared Documents/06- Real time Alert of HP Document Revs/Everest Playground/Folder Creation - Willy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoelwill\Documents\UiPath\.repositories\Everest Git\Folder Creation - Willy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{472881D3-8293-4C1A-B8EF-34C858409D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B34DC41-594A-4B5C-B97F-2F5145249251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="4" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="150" yWindow="450" windowWidth="18340" windowHeight="8570" firstSheet="4" activeTab="4" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
@@ -34,14 +34,11 @@
     <definedName name="DatePlusWorkingDays">Date!$B$9</definedName>
     <definedName name="DateText">Date!$B$19</definedName>
     <definedName name="Days">Date!$B$7</definedName>
+    <definedName name="File_Name_No_Ext">File!$B$13</definedName>
+    <definedName name="File_Name_No_Ext_No_Rev">File!$B$12</definedName>
     <definedName name="FileExtension">File!$B$10</definedName>
     <definedName name="FileName">File!$B$8</definedName>
-    <definedName name="FileNameNoExtension">File!$B$13</definedName>
-    <definedName name="FileNoextNoRev">File!$B$12</definedName>
     <definedName name="FirstName">Text!$B$15</definedName>
-    <definedName name="Folder_path">File!$B$17</definedName>
-    <definedName name="Full_New_File_name">File!$B$20</definedName>
-    <definedName name="Full_New_File_Path">File!$B$21</definedName>
     <definedName name="FullFileName_Input">File!$B$6</definedName>
     <definedName name="Int">Number!$B$6</definedName>
     <definedName name="LastMonthEndDate">Date!$C$14</definedName>
@@ -52,8 +49,11 @@
     <definedName name="LastWeekSunday">Date!$D$13</definedName>
     <definedName name="Length">Text!$B$6</definedName>
     <definedName name="LowerCase">Text!$B$8</definedName>
-    <definedName name="New_DML_Name">File!$B$18</definedName>
-    <definedName name="New_SubFolder_Path">File!$B$19</definedName>
+    <definedName name="New_DML_Full_file_Name">File!$B$18</definedName>
+    <definedName name="New_DML_Full_File_Path">File!$B$19</definedName>
+    <definedName name="New_Folder_New_Full_File_Name">File!$B$21</definedName>
+    <definedName name="New_Folder_New_Full_File_Path">File!$B$22</definedName>
+    <definedName name="New_SubFolder_Path">File!$B$20</definedName>
     <definedName name="NewRevision">File!$B$15</definedName>
     <definedName name="NewRevisionFileName">File!$B$9</definedName>
     <definedName name="Number_Input">Number!$B$4</definedName>
@@ -71,7 +71,7 @@
     <definedName name="Today">Date!$B$12</definedName>
     <definedName name="Trimmed">Text!$B$5</definedName>
     <definedName name="TwoDecimals">Number!$B$7</definedName>
-    <definedName name="UniversalDMSName">File!$B$11</definedName>
+    <definedName name="UniversalDMLName">File!$B$11</definedName>
     <definedName name="UpperCase">Text!$B$7</definedName>
     <definedName name="YYYYMMDD">Date!$B$10</definedName>
   </definedNames>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="98">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>Splits a full file name to get its folder and extension</t>
-  </si>
-  <si>
-    <t>Folder</t>
   </si>
   <si>
     <t>Days</t>
@@ -360,9 +357,6 @@
     <t>CM Name</t>
   </si>
   <si>
-    <t>Universal File Name</t>
-  </si>
-  <si>
     <t>Revision N</t>
   </si>
   <si>
@@ -372,19 +366,28 @@
     <t>Reformatted File Name N+1:</t>
   </si>
   <si>
-    <t>New Folder N + 1</t>
-  </si>
-  <si>
-    <t>Full New File Path N + 1</t>
-  </si>
-  <si>
-    <t>DML N+1 Full File Path</t>
-  </si>
-  <si>
-    <t>Full New File name N + 1</t>
-  </si>
-  <si>
     <t>C:\Temp\Everest\Document masterlist\CJA\CJA Document Masterlist Everest Rev 0.xlsx</t>
+  </si>
+  <si>
+    <t>CM Folder Path</t>
+  </si>
+  <si>
+    <t>Universal DML Name</t>
+  </si>
+  <si>
+    <t>New DML Full File Name</t>
+  </si>
+  <si>
+    <t>New DML Full File Path</t>
+  </si>
+  <si>
+    <t>New SubFolder Path</t>
+  </si>
+  <si>
+    <t>New Folder New Full File Name</t>
+  </si>
+  <si>
+    <t>New Folder New Full File Path</t>
   </si>
 </sst>
 </file>
@@ -1588,7 +1591,7 @@
     </row>
     <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
@@ -1608,15 +1611,15 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
         <v>82</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1624,7 +1627,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="26" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
@@ -1633,7 +1636,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="26" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
@@ -1834,7 +1837,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" t="str">
         <f>preferred_date_format</f>
@@ -1894,7 +1897,7 @@
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -1907,19 +1910,19 @@
         <v>54</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1931,13 +1934,13 @@
         <v>John C. Doe</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D5,Text_Input)+LEN(D5), IFERROR(FIND(IF(E5="",CHAR(10),E5),Text_Input,FIND(D5,Text_Input)+LEN(D5)),LEN(Text_Input)+1)-FIND(D5,Text_Input)-LEN(D5)))</f>
@@ -1953,7 +1956,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -1972,10 +1975,10 @@
         <v>JOHN C. DOE</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D7,Text_Input)+LEN(D7), IFERROR(FIND(IF(E7="",CHAR(10),E7),Text_Input,FIND(D7,Text_Input)+LEN(D7)),LEN(Text_Input)+1)-FIND(D7,Text_Input)-LEN(D7)))</f>
@@ -1991,10 +1994,10 @@
         <v>john c. doe</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D8,Text_Input)+LEN(D8), IFERROR(FIND(IF(E8="",CHAR(10),E8),Text_Input,FIND(D8,Text_Input)+LEN(D8)),LEN(Text_Input)+1)-FIND(D8,Text_Input)-LEN(D8)))</f>
@@ -2003,7 +2006,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="15" t="str">
         <f>TRIM(MID(Text_Input, FIND(D9,Text_Input)+LEN(D9), IFERROR(FIND(IF(E9="",CHAR(10),E9),Text_Input,FIND(D9,Text_Input)+LEN(D9)),LEN(Text_Input)+1)-FIND(D9,Text_Input)-LEN(D9)))</f>
@@ -2018,7 +2021,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -2029,7 +2032,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2041,7 +2044,7 @@
         <v>Mary C. Doe</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2053,12 +2056,12 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -2070,7 +2073,7 @@
         <v>John C.</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -2082,12 +2085,12 @@
         <v>Doe</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2126,7 +2129,7 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="24"/>
@@ -2148,7 +2151,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5">
         <f>VALUE(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Number_Input, CHAR(13), ""), CHAR(10), ""), CHAR(160), "")))</f>
@@ -2239,22 +2242,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B15AA95-D2AA-4AD6-8E83-DBFAD20B8498}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" customWidth="1"/>
-    <col min="2" max="2" width="143.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="96.36328125" customWidth="1"/>
     <col min="3" max="4" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="25"/>
@@ -2262,7 +2265,7 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="24"/>
@@ -2291,7 +2294,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -2311,10 +2314,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" t="str">
-        <f>CMName&amp;" "&amp;UniversalDMSName&amp;NewRevision&amp;"."&amp;FileExtension</f>
+        <f>CMName&amp;" "&amp;UniversalDMLName&amp;NewRevision&amp;"."&amp;FileExtension</f>
         <v>CJA Document Masterlist Everest Rev 1.xlsx</v>
       </c>
     </row>
@@ -2329,16 +2332,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="34" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B11" s="33" t="str">
-        <f>RIGHT(FileNoextNoRev, LEN(FileNoextNoRev)-4)</f>
+        <f>RIGHT(File_Name_No_Ext_No_Rev, LEN(File_Name_No_Ext_No_Rev)-4)</f>
         <v xml:space="preserve">Document Masterlist Everest Rev </v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="33" t="str">
         <f>LEFT(FileName,36)</f>
@@ -2356,7 +2359,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14" s="33" t="str">
         <f>RIGHT(B13, LEN(B13)-LEN(B12))</f>
@@ -2365,7 +2368,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" s="35">
         <f>B14+1</f>
@@ -2374,16 +2377,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="35" t="str">
-        <f>LEFT(FileNoextNoRev,3)</f>
+        <f>LEFT(File_Name_No_Ext_No_Rev,3)</f>
         <v>CJA</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="34" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B17" s="33" t="str">
         <f>LEFT(B6, LEN(B6)-LEN(B8))</f>
@@ -2392,37 +2395,46 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="37" t="str">
-        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;UniversalDMSName&amp;" "&amp;NewRevision&amp;"."&amp;FileExtension</f>
-        <v>C:\Temp\Everest\Document masterlist\CJA\Document Masterlist Everest Rev  1.xlsx</v>
+        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;File_Name_No_Ext_No_Rev&amp;NewRevision</f>
+        <v>C:\Temp\Everest\Document masterlist\CJA\CJA Document Masterlist Everest Rev 1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="33" t="str">
+        <v>94</v>
+      </c>
+      <c r="B19" s="37" t="str">
+        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;File_Name_No_Ext_No_Rev&amp;NewRevision&amp;"."&amp;FileExtension</f>
+        <v>C:\Temp\Everest\Document masterlist\CJA\CJA Document Masterlist Everest Rev 1.xlsx</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="33" t="str">
         <f>LEFT(B6, LEN(B6)-LEN(B8))&amp;"Everest Download Rev "&amp;NewRevision&amp;"\"</f>
         <v>C:\Temp\Everest\Document masterlist\CJA\Everest Download Rev 1\</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="37" t="str">
-        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;"Everest Download Rev "&amp;NewRevision&amp;"\"&amp;CMName&amp;" "&amp;UniversalDMSName&amp;NewRevision</f>
-        <v>C:\Temp\Everest\Document masterlist\CJA\Everest Download Rev 1\CJA Document Masterlist Everest Rev 1</v>
-      </c>
-    </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B21" s="37" t="str">
-        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;"Everest Download Rev "&amp;NewRevision&amp;"\"&amp;CMName&amp;" "&amp;UniversalDMSName&amp;NewRevision&amp;"."&amp;FileExtension</f>
+        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;"Everest Download Rev "&amp;NewRevision&amp;"\"&amp;CMName&amp;" "&amp;UniversalDMLName&amp;NewRevision</f>
+        <v>C:\Temp\Everest\Document masterlist\CJA\Everest Download Rev 1\CJA Document Masterlist Everest Rev 1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="37" t="str">
+        <f>LEFT(B$6, LEN(B$6)-LEN(B$8))&amp;"Everest Download Rev "&amp;NewRevision&amp;"\"&amp;CMName&amp;" "&amp;UniversalDMLName&amp;NewRevision&amp;"."&amp;FileExtension</f>
         <v>C:\Temp\Everest\Document masterlist\CJA\Everest Download Rev 1\CJA Document Masterlist Everest Rev 1.xlsx</v>
       </c>
     </row>
@@ -2457,12 +2469,12 @@
     </row>
     <row r="2" spans="1:5" ht="35" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="37" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2471,18 +2483,18 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2532,27 +2544,27 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2563,6 +2575,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5f977c50-2d7a-484c-acbd-eec5a0379d47" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6a4c4680-0984-45cb-bb92-415d6e515dfa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B16600BB3F787049B388C7CFD7EEE15C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1a82d70544a00a602877de68251abad3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6a4c4680-0984-45cb-bb92-415d6e515dfa" xmlns:ns3="5f977c50-2d7a-484c-acbd-eec5a0379d47" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bed718036c05bd3ccaa54d95c4edc461" ns2:_="" ns3:_="">
     <xsd:import namespace="6a4c4680-0984-45cb-bb92-415d6e515dfa"/>
@@ -2785,34 +2817,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5f977c50-2d7a-484c-acbd-eec5a0379d47" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6a4c4680-0984-45cb-bb92-415d6e515dfa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52D1FA1-5952-4DF9-A5CA-1242A1BDF162}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{866B838F-E4C8-4E67-B277-878368C882B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5f977c50-2d7a-484c-acbd-eec5a0379d47"/>
+    <ds:schemaRef ds:uri="6a4c4680-0984-45cb-bb92-415d6e515dfa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22DAA5A9-0921-4152-878F-F50DC19F8379}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22DAA5A9-0921-4152-878F-F50DC19F8379}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{866B838F-E4C8-4E67-B277-878368C882B9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52D1FA1-5952-4DF9-A5CA-1242A1BDF162}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6a4c4680-0984-45cb-bb92-415d6e515dfa"/>
+    <ds:schemaRef ds:uri="5f977c50-2d7a-484c-acbd-eec5a0379d47"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>